<commit_message>
adding data to 2.13
</commit_message>
<xml_diff>
--- a/BulunTe_IphoneMonitor.xlsx
+++ b/BulunTe_IphoneMonitor.xlsx
@@ -1,25 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AltanGadasTbl\Documents\Biostat620_G08\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5A76EA-FDB3-4B13-A601-F5A58822FA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -346,13 +361,109 @@
   </si>
   <si>
     <t>procrastination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>59min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2h12min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>53min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>38min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h10min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>43min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h29min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h16min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h27min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h7min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>41min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h14min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>56min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h31min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h2min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2h3min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h8min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -711,18 +822,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1835,7 +1946,7 @@
         <v>10</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18:E28" si="2">IF(ISERROR(FIND("h", D18)), 0, LEFT(D18, FIND("h", D18)-1)*60) + IF(ISERROR(FIND("min", D18)), 0, MID(D18, IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1), FIND("min", D18) - IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1)))</f>
+        <f t="shared" ref="E18:E46" si="2">IF(ISERROR(FIND("h", D18)), 0, LEFT(D18, FIND("h", D18)-1)*60) + IF(ISERROR(FIND("min", D18)), 0, MID(D18, IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1), FIND("min", D18) - IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1)))</f>
         <v>63</v>
       </c>
       <c r="F18">
@@ -2020,7 +2131,7 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:C28" si="3">IF(ISERROR(FIND("h", B21)), 0, LEFT(B21, FIND("h", B21)-1)*60) + IF(ISERROR(FIND("min", B21)), 0, MID(B21, IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1), FIND("min", B21) - IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1)))</f>
+        <f t="shared" ref="C21:C46" si="3">IF(ISERROR(FIND("h", B21)), 0, LEFT(B21, FIND("h", B21)-1)*60) + IF(ISERROR(FIND("min", B21)), 0, MID(B21, IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1), FIND("min", B21) - IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1)))</f>
         <v>31</v>
       </c>
       <c r="D21" t="s">
@@ -2521,6 +2632,1158 @@
         <v>5</v>
       </c>
       <c r="T28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>45318</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="F29">
+        <v>34</v>
+      </c>
+      <c r="G29" s="1">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>24</v>
+      </c>
+      <c r="N29">
+        <v>14.5</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>6</v>
+      </c>
+      <c r="S29">
+        <v>5</v>
+      </c>
+      <c r="T29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>45319</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>31</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>24</v>
+      </c>
+      <c r="N30">
+        <v>14.5</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>6</v>
+      </c>
+      <c r="S30">
+        <v>5</v>
+      </c>
+      <c r="T30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>45320</v>
+      </c>
+      <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="3"/>
+        <v>132</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="F31">
+        <v>76</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.32222222222222224</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>24</v>
+      </c>
+      <c r="N31">
+        <v>14.5</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>6</v>
+      </c>
+      <c r="S31">
+        <v>5</v>
+      </c>
+      <c r="T31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>45321</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="D32" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="F32">
+        <v>85</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.32013888888888892</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>24</v>
+      </c>
+      <c r="N32">
+        <v>14.5</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>6</v>
+      </c>
+      <c r="S32">
+        <v>5</v>
+      </c>
+      <c r="T32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="D33" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="F33">
+        <v>57</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2.1527777777777781E-2</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>24</v>
+      </c>
+      <c r="N33">
+        <v>14.5</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>6</v>
+      </c>
+      <c r="S33">
+        <v>5</v>
+      </c>
+      <c r="T33">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>45323</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F34">
+        <v>84</v>
+      </c>
+      <c r="G34" s="1">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>24</v>
+      </c>
+      <c r="N34">
+        <v>14.5</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>6</v>
+      </c>
+      <c r="S34">
+        <v>5</v>
+      </c>
+      <c r="T34">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>45324</v>
+      </c>
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="F35">
+        <v>43</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>24</v>
+      </c>
+      <c r="N35">
+        <v>14.5</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>6</v>
+      </c>
+      <c r="S35">
+        <v>5</v>
+      </c>
+      <c r="T35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>45325</v>
+      </c>
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F36">
+        <v>20</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.34097222222222223</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>24</v>
+      </c>
+      <c r="N36">
+        <v>14.5</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>6</v>
+      </c>
+      <c r="S36">
+        <v>5</v>
+      </c>
+      <c r="T36">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>45326</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>23</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.30763888888888891</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>24</v>
+      </c>
+      <c r="N37">
+        <v>14.5</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>6</v>
+      </c>
+      <c r="S37">
+        <v>5</v>
+      </c>
+      <c r="T37">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>45327</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F38">
+        <v>59</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>24</v>
+      </c>
+      <c r="N38">
+        <v>14.5</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>6</v>
+      </c>
+      <c r="S38">
+        <v>5</v>
+      </c>
+      <c r="T38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>45328</v>
+      </c>
+      <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="D39" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="F39">
+        <v>63</v>
+      </c>
+      <c r="G39" s="1">
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>24</v>
+      </c>
+      <c r="N39">
+        <v>14.5</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>6</v>
+      </c>
+      <c r="S39">
+        <v>5</v>
+      </c>
+      <c r="T39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>45329</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <v>70</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>24</v>
+      </c>
+      <c r="N40">
+        <v>14.5</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>6</v>
+      </c>
+      <c r="S40">
+        <v>5</v>
+      </c>
+      <c r="T40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="D41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41">
+        <f>IF(ISERROR(FIND("h", D41)), 0, LEFT(D41, FIND("h", D41)-1)*60) + IF(ISERROR(FIND("min", D41)), 0, MID(D41, IF(ISERROR(FIND("h", D41)), 1, FIND("h", D41)+1), FIND("min", D41) - IF(ISERROR(FIND("h", D41)), 1, FIND("h", D41)+1)))</f>
+        <v>87</v>
+      </c>
+      <c r="F41">
+        <v>78</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.31875000000000003</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>24</v>
+      </c>
+      <c r="N41">
+        <v>14.5</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>6</v>
+      </c>
+      <c r="S41">
+        <v>5</v>
+      </c>
+      <c r="T41">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="D42" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="F42">
+        <v>87</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.20416666666666669</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>24</v>
+      </c>
+      <c r="N42">
+        <v>14.5</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>6</v>
+      </c>
+      <c r="S42">
+        <v>5</v>
+      </c>
+      <c r="T42">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>45332</v>
+      </c>
+      <c r="B43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="D43" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="F43">
+        <v>34</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.30416666666666664</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>24</v>
+      </c>
+      <c r="N43">
+        <v>14.5</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>6</v>
+      </c>
+      <c r="S43">
+        <v>5</v>
+      </c>
+      <c r="T43">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>45333</v>
+      </c>
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="F44">
+        <v>34</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.3215277777777778</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>24</v>
+      </c>
+      <c r="N44">
+        <v>14.5</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>6</v>
+      </c>
+      <c r="S44">
+        <v>5</v>
+      </c>
+      <c r="T44">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>45334</v>
+      </c>
+      <c r="B45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="D45" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="F45">
+        <v>66</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>24</v>
+      </c>
+      <c r="N45">
+        <v>14.5</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>6</v>
+      </c>
+      <c r="S45">
+        <v>5</v>
+      </c>
+      <c r="T45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>45335</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="3"/>
+        <v>123</v>
+      </c>
+      <c r="D46" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="F46">
+        <v>43</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.32916666666666666</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>24</v>
+      </c>
+      <c r="N46">
+        <v>14.5</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>6</v>
+      </c>
+      <c r="S46">
+        <v>5</v>
+      </c>
+      <c r="T46">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reformating dates and creating RData
</commit_message>
<xml_diff>
--- a/BulunTe_IphoneMonitor.xlsx
+++ b/BulunTe_IphoneMonitor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AltanGadasTbl\Documents\Biostat620_G08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5A76EA-FDB3-4B13-A601-F5A58822FA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450BDD11-A406-4444-ABE6-EB70CBA090D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,42 +55,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1/16/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2h24min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1/17/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1h3min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1/18/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1/19/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1/20/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1/21/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1/22/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2h32min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -128,14 +91,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1/25/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1/24/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1h34min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -144,18 +99,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1/23/24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4h5min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>12/31/23</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>30min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -297,10 +244,6 @@
   </si>
   <si>
     <t>58min</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1/26/24</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -464,9 +407,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="m/d/yy;@"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -513,7 +453,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -832,13 +772,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.125" bestFit="1" customWidth="1"/>
@@ -868,58 +808,58 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" t="s">
-        <v>80</v>
-      </c>
-      <c r="T1" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
+      <c r="A2" s="2">
+        <v>45291</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C17" si="0">IF(ISERROR(FIND("h", B2)), 0, LEFT(B2, FIND("h", B2)-1)*60) + IF(ISERROR(FIND("min", B2)), 0, MID(B2, IF(ISERROR(FIND("h", B2)), 1, FIND("h", B2)+1), FIND("min", B2) - IF(ISERROR(FIND("h", B2)), 1, FIND("h", B2)+1)))</f>
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E17" si="1">IF(ISERROR(FIND("h", D2)), 0, LEFT(D2, FIND("h", D2)-1)*60) + IF(ISERROR(FIND("min", D2)), 0, MID(D2, IF(ISERROR(FIND("h", D2)), 1, FIND("h", D2)+1), FIND("min", D2) - IF(ISERROR(FIND("h", D2)), 1, FIND("h", D2)+1)))</f>
@@ -976,14 +916,14 @@
         <v>45292</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
@@ -1040,14 +980,14 @@
         <v>45293</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
@@ -1104,14 +1044,14 @@
         <v>45294</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
@@ -1168,14 +1108,14 @@
         <v>45295</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
@@ -1232,14 +1172,14 @@
         <v>45296</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
@@ -1296,14 +1236,14 @@
         <v>45297</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
@@ -1360,14 +1300,14 @@
         <v>45298</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
@@ -1424,14 +1364,14 @@
         <v>45299</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
@@ -1488,14 +1428,14 @@
         <v>45300</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
@@ -1552,14 +1492,14 @@
         <v>45301</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
@@ -1616,14 +1556,14 @@
         <v>45302</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
@@ -1680,14 +1620,14 @@
         <v>45303</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
@@ -1744,14 +1684,14 @@
         <v>45304</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
         <v>129</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
@@ -1808,14 +1748,14 @@
         <v>45305</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
@@ -1872,14 +1812,14 @@
         <v>45306</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
         <v>146</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
@@ -1932,18 +1872,18 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="2">
+        <v>45307</v>
+      </c>
+      <c r="B18" t="s">
         <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
       </c>
       <c r="C18">
         <f>IF(ISERROR(FIND("h", B18)), 0, LEFT(B18, FIND("h", B18)-1)*60) + IF(ISERROR(FIND("min", B18)), 0, MID(B18, IF(ISERROR(FIND("h", B18)), 1, FIND("h", B18)+1), FIND("min", B18) - IF(ISERROR(FIND("h", B18)), 1, FIND("h", B18)+1)))</f>
         <v>144</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E18">
         <f t="shared" ref="E18:E46" si="2">IF(ISERROR(FIND("h", D18)), 0, LEFT(D18, FIND("h", D18)-1)*60) + IF(ISERROR(FIND("min", D18)), 0, MID(D18, IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1), FIND("min", D18) - IF(ISERROR(FIND("h", D18)), 1, FIND("h", D18)+1)))</f>
@@ -1996,18 +1936,18 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>9</v>
+      <c r="A19" s="2">
+        <v>45308</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C19">
         <f>IF(ISERROR(FIND("h", B19)), 0, LEFT(B19, FIND("h", B19)-1)*60) + IF(ISERROR(FIND("min", B19)), 0, MID(B19, IF(ISERROR(FIND("h", B19)), 1, FIND("h", B19)+1), FIND("min", B19) - IF(ISERROR(FIND("h", B19)), 1, FIND("h", B19)+1)))</f>
         <v>163</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
@@ -2060,18 +2000,18 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>11</v>
+      <c r="A20" s="2">
+        <v>45309</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <f>IF(ISERROR(FIND("h", B20)), 0, LEFT(B20, FIND("h", B20)-1)*60) + IF(ISERROR(FIND("min", B20)), 0, MID(B20, IF(ISERROR(FIND("h", B20)), 1, FIND("h", B20)+1), FIND("min", B20) - IF(ISERROR(FIND("h", B20)), 1, FIND("h", B20)+1)))</f>
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
@@ -2124,18 +2064,18 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="2">
+        <v>45310</v>
+      </c>
+      <c r="B21" t="s">
         <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
       </c>
       <c r="C21">
         <f t="shared" ref="C21:C46" si="3">IF(ISERROR(FIND("h", B21)), 0, LEFT(B21, FIND("h", B21)-1)*60) + IF(ISERROR(FIND("min", B21)), 0, MID(B21, IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1), FIND("min", B21) - IF(ISERROR(FIND("h", B21)), 1, FIND("h", B21)+1)))</f>
         <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
@@ -2188,18 +2128,18 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>13</v>
+      <c r="A22" s="2">
+        <v>45311</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C22">
         <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
@@ -2252,18 +2192,18 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>14</v>
+      <c r="A23" s="2">
+        <v>45312</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <f t="shared" si="3"/>
         <v>222</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
@@ -2316,18 +2256,18 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>15</v>
+      <c r="A24" s="2">
+        <v>45313</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <f t="shared" si="3"/>
         <v>152</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
@@ -2380,18 +2320,18 @@
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>27</v>
+      <c r="A25" s="2">
+        <v>45314</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <f t="shared" si="3"/>
         <v>245</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
@@ -2444,18 +2384,18 @@
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>24</v>
+      <c r="A26" s="2">
+        <v>45315</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C26">
         <f t="shared" si="3"/>
         <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
@@ -2508,18 +2448,18 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>23</v>
+      <c r="A27" s="2">
+        <v>45316</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C27">
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E27">
         <f t="shared" si="2"/>
@@ -2572,18 +2512,18 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>66</v>
+      <c r="A28" s="2">
+        <v>45317</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C28">
         <f t="shared" si="3"/>
         <v>333</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E28">
         <f t="shared" si="2"/>
@@ -2640,14 +2580,14 @@
         <v>45318</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C29">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E29">
         <f t="shared" si="2"/>
@@ -2704,14 +2644,14 @@
         <v>45319</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C30">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
@@ -2768,14 +2708,14 @@
         <v>45320</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C31">
         <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E31">
         <f t="shared" si="2"/>
@@ -2832,14 +2772,14 @@
         <v>45321</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C32">
         <f t="shared" si="3"/>
         <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E32">
         <f t="shared" si="2"/>
@@ -2896,14 +2836,14 @@
         <v>45322</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C33">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E33">
         <f t="shared" si="2"/>
@@ -2960,14 +2900,14 @@
         <v>45323</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C34">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E34">
         <f t="shared" si="2"/>
@@ -3024,14 +2964,14 @@
         <v>45324</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C35">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E35">
         <f t="shared" si="2"/>
@@ -3088,14 +3028,14 @@
         <v>45325</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C36">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E36">
         <f t="shared" si="2"/>
@@ -3152,14 +3092,14 @@
         <v>45326</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C37">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E37">
         <f t="shared" si="2"/>
@@ -3216,14 +3156,14 @@
         <v>45327</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C38">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E38">
         <f t="shared" si="2"/>
@@ -3280,14 +3220,14 @@
         <v>45328</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C39">
         <f t="shared" si="3"/>
         <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E39">
         <f t="shared" si="2"/>
@@ -3344,14 +3284,14 @@
         <v>45329</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C40">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E40">
         <f t="shared" si="2"/>
@@ -3408,14 +3348,14 @@
         <v>45330</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C41">
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E41">
         <f>IF(ISERROR(FIND("h", D41)), 0, LEFT(D41, FIND("h", D41)-1)*60) + IF(ISERROR(FIND("min", D41)), 0, MID(D41, IF(ISERROR(FIND("h", D41)), 1, FIND("h", D41)+1), FIND("min", D41) - IF(ISERROR(FIND("h", D41)), 1, FIND("h", D41)+1)))</f>
@@ -3472,14 +3412,14 @@
         <v>45331</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C42">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
       <c r="D42" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E42">
         <f t="shared" si="2"/>
@@ -3536,14 +3476,14 @@
         <v>45332</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C43">
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E43">
         <f t="shared" si="2"/>
@@ -3600,14 +3540,14 @@
         <v>45333</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C44">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E44">
         <f t="shared" si="2"/>
@@ -3664,14 +3604,14 @@
         <v>45334</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C45">
         <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E45">
         <f t="shared" si="2"/>
@@ -3728,14 +3668,14 @@
         <v>45335</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C46">
         <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E46">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
adding temperature and steps, upgrading data
</commit_message>
<xml_diff>
--- a/BulunTe_IphoneMonitor.xlsx
+++ b/BulunTe_IphoneMonitor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AltanGadasTbl\Documents\Biostat620_G08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450BDD11-A406-4444-ABE6-EB70CBA090D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1653B81-3A84-4D21-AF0F-3D2AE36E1987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -400,6 +409,20 @@
   </si>
   <si>
     <t>1h8min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Temperature_F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temperature_C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,6 +430,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,7 +472,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -455,6 +481,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -781,11 +810,14 @@
     <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -807,47 +839,59 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>59</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>60</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>61</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>62</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>63</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>64</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>66</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>67</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>68</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="X1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45291</v>
       </c>
@@ -871,47 +915,59 @@
       <c r="G2" s="1">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
+      <c r="H2" s="3">
+        <v>34</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="J2" s="3">
         <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>6</v>
+      </c>
+      <c r="V2">
+        <v>5</v>
+      </c>
+      <c r="W2">
+        <v>25</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45292</v>
       </c>
@@ -935,47 +991,59 @@
       <c r="G3" s="1">
         <v>0.16805555555555554</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+      <c r="H3" s="3">
+        <v>31</v>
+      </c>
+      <c r="I3" s="3">
+        <v>-0.55555555555555558</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>6</v>
+      </c>
+      <c r="V3">
+        <v>5</v>
+      </c>
+      <c r="W3">
+        <v>25</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45293</v>
       </c>
@@ -999,47 +1067,59 @@
       <c r="G4" s="1">
         <v>0.29791666666666666</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
+      <c r="H4" s="3">
+        <v>30</v>
+      </c>
+      <c r="I4" s="3">
+        <v>-1.1111111111111112</v>
+      </c>
+      <c r="J4" s="3">
         <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>6</v>
+      </c>
+      <c r="V4">
+        <v>5</v>
+      </c>
+      <c r="W4">
+        <v>25</v>
+      </c>
+      <c r="X4">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45294</v>
       </c>
@@ -1063,47 +1143,59 @@
       <c r="G5" s="1">
         <v>0.31944444444444448</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
+      <c r="H5" s="3">
+        <v>32</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
         <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>6</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <v>25</v>
+      </c>
+      <c r="X5">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45295</v>
       </c>
@@ -1127,47 +1219,59 @@
       <c r="G6" s="1">
         <v>0.375</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
+      <c r="H6" s="3">
+        <v>20</v>
+      </c>
+      <c r="I6" s="3">
+        <v>-6.6666666666666661</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>6</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="W6">
+        <v>25</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45296</v>
       </c>
@@ -1191,47 +1295,59 @@
       <c r="G7" s="1">
         <v>0.375</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
+      <c r="H7" s="3">
+        <v>19</v>
+      </c>
+      <c r="I7" s="3">
+        <v>-7.2222222222222223</v>
+      </c>
+      <c r="J7" s="3">
         <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+      <c r="V7">
+        <v>5</v>
+      </c>
+      <c r="W7">
+        <v>25</v>
+      </c>
+      <c r="X7">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45297</v>
       </c>
@@ -1255,47 +1371,59 @@
       <c r="G8" s="1">
         <v>0.33402777777777781</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
+      <c r="H8" s="3">
+        <v>28</v>
+      </c>
+      <c r="I8" s="3">
+        <v>-2.2222222222222223</v>
+      </c>
+      <c r="J8" s="3">
         <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+      <c r="W8">
+        <v>25</v>
+      </c>
+      <c r="X8">
+        <v>6246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45298</v>
       </c>
@@ -1319,47 +1447,59 @@
       <c r="G9" s="1">
         <v>0.30972222222222223</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
+      <c r="H9" s="3">
+        <v>30</v>
+      </c>
+      <c r="I9" s="3">
+        <v>-1.1111111111111112</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R9">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="W9">
+        <v>25</v>
+      </c>
+      <c r="X9">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45299</v>
       </c>
@@ -1383,47 +1523,59 @@
       <c r="G10" s="1">
         <v>3.9583333333333331E-2</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
+      <c r="H10" s="3">
+        <v>32</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>6</v>
+      </c>
+      <c r="V10">
+        <v>5</v>
+      </c>
+      <c r="W10">
+        <v>25</v>
+      </c>
+      <c r="X10">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45300</v>
       </c>
@@ -1447,47 +1599,59 @@
       <c r="G11" s="1">
         <v>0.33749999999999997</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
+      <c r="H11" s="3">
+        <v>33</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R11">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>6</v>
+      </c>
+      <c r="V11">
+        <v>5</v>
+      </c>
+      <c r="W11">
+        <v>25</v>
+      </c>
+      <c r="X11">
+        <v>4838</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45301</v>
       </c>
@@ -1511,47 +1675,59 @@
       <c r="G12" s="1">
         <v>0.3125</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
+      <c r="H12" s="3">
+        <v>33</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>6</v>
+      </c>
+      <c r="V12">
+        <v>5</v>
+      </c>
+      <c r="W12">
+        <v>25</v>
+      </c>
+      <c r="X12">
+        <v>8460</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45302</v>
       </c>
@@ -1575,47 +1751,59 @@
       <c r="G13" s="1">
         <v>6.5277777777777782E-2</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
+      <c r="H13" s="3">
+        <v>30</v>
+      </c>
+      <c r="I13" s="3">
+        <v>-1.1111111111111112</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>6</v>
+      </c>
+      <c r="V13">
+        <v>5</v>
+      </c>
+      <c r="W13">
+        <v>25</v>
+      </c>
+      <c r="X13">
+        <v>6670</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45303</v>
       </c>
@@ -1639,47 +1827,59 @@
       <c r="G14" s="1">
         <v>0.4069444444444445</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
+      <c r="H14" s="3">
+        <v>30</v>
+      </c>
+      <c r="I14" s="3">
+        <v>-1.1111111111111112</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>6</v>
+      </c>
+      <c r="V14">
+        <v>5</v>
+      </c>
+      <c r="W14">
+        <v>25</v>
+      </c>
+      <c r="X14">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45304</v>
       </c>
@@ -1703,47 +1903,59 @@
       <c r="G15" s="1">
         <v>4.6527777777777779E-2</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
+      <c r="H15" s="3">
+        <v>17</v>
+      </c>
+      <c r="I15" s="3">
+        <v>-8.3333333333333339</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>6</v>
+      </c>
+      <c r="V15">
+        <v>5</v>
+      </c>
+      <c r="W15">
+        <v>25</v>
+      </c>
+      <c r="X15">
+        <v>4961</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>45305</v>
       </c>
@@ -1767,47 +1979,59 @@
       <c r="G16" s="1">
         <v>0.33749999999999997</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
+      <c r="H16" s="3">
+        <v>-2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>-18.888888888888889</v>
+      </c>
+      <c r="J16" s="3">
         <v>0</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>6</v>
+      </c>
+      <c r="V16">
+        <v>5</v>
+      </c>
+      <c r="W16">
+        <v>25</v>
+      </c>
+      <c r="X16">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>45306</v>
       </c>
@@ -1831,47 +2055,59 @@
       <c r="G17" s="1">
         <v>0.15347222222222223</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
+      <c r="H17" s="3">
+        <v>-3</v>
+      </c>
+      <c r="I17" s="3">
+        <v>-19.444444444444443</v>
+      </c>
+      <c r="J17" s="3">
         <v>0</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>6</v>
+      </c>
+      <c r="V17">
+        <v>5</v>
+      </c>
+      <c r="W17">
+        <v>25</v>
+      </c>
+      <c r="X17">
+        <v>3577</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>45307</v>
       </c>
@@ -1895,47 +2131,59 @@
       <c r="G18" s="1">
         <v>0.29791666666666666</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
+      <c r="H18" s="3">
+        <v>3</v>
+      </c>
+      <c r="I18" s="3">
+        <v>-16.111111111111111</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R18">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>6</v>
+      </c>
+      <c r="V18">
+        <v>5</v>
+      </c>
+      <c r="W18">
+        <v>25</v>
+      </c>
+      <c r="X18">
+        <v>8836</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>45308</v>
       </c>
@@ -1959,47 +2207,59 @@
       <c r="G19" s="1">
         <v>0.30486111111111108</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
+      <c r="H19" s="3">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3">
+        <v>-16.666666666666668</v>
+      </c>
+      <c r="J19" s="3">
         <v>0</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S19">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>6</v>
+      </c>
+      <c r="V19">
+        <v>5</v>
+      </c>
+      <c r="W19">
+        <v>25</v>
+      </c>
+      <c r="X19">
+        <v>13418</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>45309</v>
       </c>
@@ -2023,47 +2283,59 @@
       <c r="G20" s="1">
         <v>0.3034722222222222</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
+      <c r="H20" s="3">
+        <v>18</v>
+      </c>
+      <c r="I20" s="3">
+        <v>-7.7777777777777777</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R20">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S20">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T20">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>6</v>
+      </c>
+      <c r="V20">
+        <v>5</v>
+      </c>
+      <c r="W20">
+        <v>25</v>
+      </c>
+      <c r="X20">
+        <v>7654</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>45310</v>
       </c>
@@ -2087,47 +2359,59 @@
       <c r="G21" s="1">
         <v>0.3</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
+      <c r="H21" s="3">
+        <v>9</v>
+      </c>
+      <c r="I21" s="3">
+        <v>-12.777777777777777</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R21">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T21">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>6</v>
+      </c>
+      <c r="V21">
+        <v>5</v>
+      </c>
+      <c r="W21">
+        <v>25</v>
+      </c>
+      <c r="X21">
+        <v>7171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>45311</v>
       </c>
@@ -2151,47 +2435,59 @@
       <c r="G22" s="1">
         <v>1.5277777777777777E-2</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
+      <c r="H22" s="3">
+        <v>2</v>
+      </c>
+      <c r="I22" s="3">
+        <v>-16.666666666666668</v>
+      </c>
+      <c r="J22" s="3">
+        <v>1</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R22">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T22">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>6</v>
+      </c>
+      <c r="V22">
+        <v>5</v>
+      </c>
+      <c r="W22">
+        <v>25</v>
+      </c>
+      <c r="X22">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>45312</v>
       </c>
@@ -2215,47 +2511,59 @@
       <c r="G23" s="1">
         <v>7.6388888888888886E-3</v>
       </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
+      <c r="H23" s="3">
+        <v>8</v>
+      </c>
+      <c r="I23" s="3">
+        <v>-13.333333333333332</v>
+      </c>
+      <c r="J23" s="3">
         <v>0</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N23">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T23">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>6</v>
+      </c>
+      <c r="V23">
+        <v>5</v>
+      </c>
+      <c r="W23">
+        <v>25</v>
+      </c>
+      <c r="X23">
+        <v>4517</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>45313</v>
       </c>
@@ -2279,47 +2587,59 @@
       <c r="G24" s="1">
         <v>0.30694444444444441</v>
       </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
+      <c r="H24" s="3">
+        <v>11</v>
+      </c>
+      <c r="I24" s="3">
+        <v>-11.666666666666668</v>
+      </c>
+      <c r="J24" s="3">
         <v>0</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N24">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R24">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S24">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T24">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>6</v>
+      </c>
+      <c r="V24">
+        <v>5</v>
+      </c>
+      <c r="W24">
+        <v>25</v>
+      </c>
+      <c r="X24">
+        <v>7927</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>45314</v>
       </c>
@@ -2343,47 +2663,59 @@
       <c r="G25" s="1">
         <v>0.31458333333333333</v>
       </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
+      <c r="H25" s="3">
+        <v>32</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>1</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N25">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R25">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S25">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T25">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>6</v>
+      </c>
+      <c r="V25">
+        <v>5</v>
+      </c>
+      <c r="W25">
+        <v>25</v>
+      </c>
+      <c r="X25">
+        <v>10019</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>45315</v>
       </c>
@@ -2407,47 +2739,59 @@
       <c r="G26" s="1">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
+      <c r="H26" s="3">
+        <v>33</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q26">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R26">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S26">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T26">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>6</v>
+      </c>
+      <c r="V26">
+        <v>5</v>
+      </c>
+      <c r="W26">
+        <v>25</v>
+      </c>
+      <c r="X26">
+        <v>5212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>45316</v>
       </c>
@@ -2471,47 +2815,59 @@
       <c r="G27" s="1">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
+      <c r="H27" s="3">
+        <v>36</v>
+      </c>
+      <c r="I27" s="3">
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N27">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R27">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S27">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>6</v>
+      </c>
+      <c r="V27">
+        <v>5</v>
+      </c>
+      <c r="W27">
+        <v>25</v>
+      </c>
+      <c r="X27">
+        <v>10203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>45317</v>
       </c>
@@ -2535,47 +2891,59 @@
       <c r="G28" s="1">
         <v>0.25</v>
       </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
+      <c r="H28" s="3">
+        <v>37</v>
+      </c>
+      <c r="I28" s="3">
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q28">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R28">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S28">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>6</v>
+      </c>
+      <c r="V28">
+        <v>5</v>
+      </c>
+      <c r="W28">
+        <v>25</v>
+      </c>
+      <c r="X28">
+        <v>8241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>45318</v>
       </c>
@@ -2599,47 +2967,59 @@
       <c r="G29" s="1">
         <v>5.486111111111111E-2</v>
       </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
+      <c r="H29" s="3">
+        <v>35</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N29">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q29">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R29">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S29">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T29">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>6</v>
+      </c>
+      <c r="V29">
+        <v>5</v>
+      </c>
+      <c r="W29">
+        <v>25</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>45319</v>
       </c>
@@ -2663,47 +3043,59 @@
       <c r="G30" s="1">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
+      <c r="H30" s="3">
+        <v>33</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J30" s="3">
+        <v>1</v>
       </c>
       <c r="K30">
         <v>0</v>
       </c>
       <c r="L30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N30">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q30">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R30">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S30">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T30">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>6</v>
+      </c>
+      <c r="V30">
+        <v>5</v>
+      </c>
+      <c r="W30">
+        <v>25</v>
+      </c>
+      <c r="X30">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>45320</v>
       </c>
@@ -2727,47 +3119,59 @@
       <c r="G31" s="1">
         <v>0.32222222222222224</v>
       </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
+      <c r="H31" s="3">
+        <v>32</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1</v>
       </c>
       <c r="K31">
         <v>0</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N31">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P31">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q31">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R31">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S31">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T31">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>6</v>
+      </c>
+      <c r="V31">
+        <v>5</v>
+      </c>
+      <c r="W31">
+        <v>25</v>
+      </c>
+      <c r="X31">
+        <v>9117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>45321</v>
       </c>
@@ -2791,47 +3195,59 @@
       <c r="G32" s="1">
         <v>0.32013888888888892</v>
       </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
+      <c r="H32" s="3">
+        <v>32</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
         <v>0</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N32">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q32">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R32">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>6</v>
+      </c>
+      <c r="V32">
+        <v>5</v>
+      </c>
+      <c r="W32">
+        <v>25</v>
+      </c>
+      <c r="X32">
+        <v>12606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>45322</v>
       </c>
@@ -2855,47 +3271,59 @@
       <c r="G33" s="1">
         <v>2.1527777777777781E-2</v>
       </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
+      <c r="H33" s="3">
+        <v>33</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J33" s="3">
+        <v>1</v>
       </c>
       <c r="K33">
         <v>0</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N33">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q33">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R33">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T33">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>6</v>
+      </c>
+      <c r="V33">
+        <v>5</v>
+      </c>
+      <c r="W33">
+        <v>25</v>
+      </c>
+      <c r="X33">
+        <v>6371</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>45323</v>
       </c>
@@ -2919,47 +3347,59 @@
       <c r="G34" s="1">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
+      <c r="H34" s="3">
+        <v>36</v>
+      </c>
+      <c r="I34" s="3">
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="J34" s="3">
         <v>0</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N34">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P34">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q34">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R34">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S34">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T34">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>6</v>
+      </c>
+      <c r="V34">
+        <v>5</v>
+      </c>
+      <c r="W34">
+        <v>25</v>
+      </c>
+      <c r="X34">
+        <v>14718</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>45324</v>
       </c>
@@ -2983,47 +3423,59 @@
       <c r="G35" s="1">
         <v>0.3125</v>
       </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
+      <c r="H35" s="3">
+        <v>30</v>
+      </c>
+      <c r="I35" s="3">
+        <v>-1.1111111111111112</v>
+      </c>
+      <c r="J35" s="3">
         <v>0</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N35">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q35">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R35">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T35">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>6</v>
+      </c>
+      <c r="V35">
+        <v>5</v>
+      </c>
+      <c r="W35">
+        <v>25</v>
+      </c>
+      <c r="X35">
+        <v>9423</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>45325</v>
       </c>
@@ -3047,47 +3499,59 @@
       <c r="G36" s="1">
         <v>0.34097222222222223</v>
       </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36">
+      <c r="H36" s="3">
+        <v>26</v>
+      </c>
+      <c r="I36" s="3">
+        <v>-3.333333333333333</v>
+      </c>
+      <c r="J36" s="3">
         <v>0</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N36">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P36">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q36">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R36">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S36">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T36">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>6</v>
+      </c>
+      <c r="V36">
+        <v>5</v>
+      </c>
+      <c r="W36">
+        <v>25</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>45326</v>
       </c>
@@ -3111,47 +3575,59 @@
       <c r="G37" s="1">
         <v>0.30763888888888891</v>
       </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
+      <c r="H37" s="3">
+        <v>24</v>
+      </c>
+      <c r="I37" s="3">
+        <v>-4.4444444444444446</v>
+      </c>
+      <c r="J37" s="3">
         <v>0</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M37">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N37">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q37">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R37">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S37">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T37">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>6</v>
+      </c>
+      <c r="V37">
+        <v>5</v>
+      </c>
+      <c r="W37">
+        <v>25</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>45327</v>
       </c>
@@ -3175,47 +3651,59 @@
       <c r="G38" s="1">
         <v>0.3125</v>
       </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
+      <c r="H38" s="3">
+        <v>26</v>
+      </c>
+      <c r="I38" s="3">
+        <v>-3.333333333333333</v>
+      </c>
+      <c r="J38" s="3">
         <v>0</v>
       </c>
       <c r="K38">
         <v>0</v>
       </c>
       <c r="L38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N38">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P38">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q38">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R38">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T38">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>6</v>
+      </c>
+      <c r="V38">
+        <v>5</v>
+      </c>
+      <c r="W38">
+        <v>25</v>
+      </c>
+      <c r="X38">
+        <v>6363</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>45328</v>
       </c>
@@ -3239,47 +3727,59 @@
       <c r="G39" s="1">
         <v>6.2499999999999995E-3</v>
       </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
+      <c r="H39" s="3">
+        <v>29</v>
+      </c>
+      <c r="I39" s="3">
+        <v>-1.6666666666666665</v>
+      </c>
+      <c r="J39" s="3">
         <v>0</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N39">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P39">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q39">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R39">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S39">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T39">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>6</v>
+      </c>
+      <c r="V39">
+        <v>5</v>
+      </c>
+      <c r="W39">
+        <v>25</v>
+      </c>
+      <c r="X39">
+        <v>7432</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>45329</v>
       </c>
@@ -3303,47 +3803,59 @@
       <c r="G40" s="1">
         <v>0</v>
       </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
+      <c r="H40" s="3">
+        <v>26</v>
+      </c>
+      <c r="I40" s="3">
+        <v>-3.333333333333333</v>
+      </c>
+      <c r="J40" s="3">
         <v>0</v>
       </c>
       <c r="K40">
         <v>0</v>
       </c>
       <c r="L40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N40">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P40">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q40">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R40">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T40">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>6</v>
+      </c>
+      <c r="V40">
+        <v>5</v>
+      </c>
+      <c r="W40">
+        <v>25</v>
+      </c>
+      <c r="X40">
+        <v>7426</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45330</v>
       </c>
@@ -3367,47 +3879,59 @@
       <c r="G41" s="1">
         <v>0.31875000000000003</v>
       </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
+      <c r="H41" s="3">
+        <v>33</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J41" s="3">
         <v>0</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N41">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P41">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q41">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R41">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S41">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T41">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>6</v>
+      </c>
+      <c r="V41">
+        <v>5</v>
+      </c>
+      <c r="W41">
+        <v>25</v>
+      </c>
+      <c r="X41">
+        <v>9287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>45331</v>
       </c>
@@ -3431,47 +3955,59 @@
       <c r="G42" s="1">
         <v>0.20416666666666669</v>
       </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
+      <c r="H42" s="3">
+        <v>49</v>
+      </c>
+      <c r="I42" s="3">
+        <v>9.4444444444444446</v>
+      </c>
+      <c r="J42" s="3">
         <v>0</v>
       </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N42">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P42">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q42">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R42">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S42">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T42">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>6</v>
+      </c>
+      <c r="V42">
+        <v>5</v>
+      </c>
+      <c r="W42">
+        <v>25</v>
+      </c>
+      <c r="X42">
+        <v>12078</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>45332</v>
       </c>
@@ -3495,47 +4031,59 @@
       <c r="G43" s="1">
         <v>0.30416666666666664</v>
       </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
+      <c r="H43" s="3">
+        <v>34</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="J43" s="3">
         <v>0</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N43">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P43">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q43">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R43">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S43">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T43">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <v>6</v>
+      </c>
+      <c r="V43">
+        <v>5</v>
+      </c>
+      <c r="W43">
+        <v>25</v>
+      </c>
+      <c r="X43">
+        <v>7404</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>45333</v>
       </c>
@@ -3559,47 +4107,59 @@
       <c r="G44" s="1">
         <v>0.3215277777777778</v>
       </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
+      <c r="H44" s="3">
+        <v>28</v>
+      </c>
+      <c r="I44" s="3">
+        <v>-2.2222222222222223</v>
+      </c>
+      <c r="J44" s="3">
         <v>0</v>
       </c>
       <c r="K44">
         <v>0</v>
       </c>
       <c r="L44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M44">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N44">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P44">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q44">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R44">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S44">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T44">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>6</v>
+      </c>
+      <c r="V44">
+        <v>5</v>
+      </c>
+      <c r="W44">
+        <v>25</v>
+      </c>
+      <c r="X44">
+        <v>5608</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45334</v>
       </c>
@@ -3623,47 +4183,59 @@
       <c r="G45" s="1">
         <v>0.3125</v>
       </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
+      <c r="H45" s="3">
+        <v>28</v>
+      </c>
+      <c r="I45" s="3">
+        <v>-2.2222222222222223</v>
+      </c>
+      <c r="J45" s="3">
         <v>0</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N45">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P45">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q45">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R45">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S45">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T45">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U45">
+        <v>6</v>
+      </c>
+      <c r="V45">
+        <v>5</v>
+      </c>
+      <c r="W45">
+        <v>25</v>
+      </c>
+      <c r="X45">
+        <v>5343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45335</v>
       </c>
@@ -3687,44 +4259,56 @@
       <c r="G46" s="1">
         <v>0.32916666666666666</v>
       </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-      <c r="J46">
+      <c r="H46" s="3">
+        <v>26</v>
+      </c>
+      <c r="I46" s="3">
+        <v>-3.333333333333333</v>
+      </c>
+      <c r="J46" s="3">
         <v>0</v>
       </c>
       <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M46">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N46">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="O46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P46">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q46">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="R46">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S46">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T46">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>6</v>
+      </c>
+      <c r="V46">
+        <v>5</v>
+      </c>
+      <c r="W46">
+        <v>25</v>
+      </c>
+      <c r="X46">
+        <v>7720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating Temperature which was chracter
</commit_message>
<xml_diff>
--- a/BulunTe_IphoneMonitor.xlsx
+++ b/BulunTe_IphoneMonitor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AltanGadasTbl\Documents\Biostat620_G08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1653B81-3A84-4D21-AF0F-3D2AE36E1987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA76A02-2E99-4D91-A726-82159C153A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -483,6 +483,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -802,7 +805,7 @@
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -810,8 +813,8 @@
     <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.25" customWidth="1"/>
@@ -839,10 +842,10 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>97</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -915,10 +918,10 @@
       <c r="G2" s="1">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>34</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="4">
         <v>1.1111111111111112</v>
       </c>
       <c r="J2" s="3">
@@ -991,10 +994,10 @@
       <c r="G3" s="1">
         <v>0.16805555555555554</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>31</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="4">
         <v>-0.55555555555555558</v>
       </c>
       <c r="J3" s="3">
@@ -1067,10 +1070,10 @@
       <c r="G4" s="1">
         <v>0.29791666666666666</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <v>30</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="4">
         <v>-1.1111111111111112</v>
       </c>
       <c r="J4" s="3">
@@ -1143,10 +1146,10 @@
       <c r="G5" s="1">
         <v>0.31944444444444448</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="4">
         <v>32</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="4">
         <v>0</v>
       </c>
       <c r="J5" s="3">
@@ -1219,10 +1222,10 @@
       <c r="G6" s="1">
         <v>0.375</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <v>20</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="4">
         <v>-6.6666666666666661</v>
       </c>
       <c r="J6" s="3">
@@ -1295,10 +1298,10 @@
       <c r="G7" s="1">
         <v>0.375</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
         <v>19</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="4">
         <v>-7.2222222222222223</v>
       </c>
       <c r="J7" s="3">
@@ -1371,10 +1374,10 @@
       <c r="G8" s="1">
         <v>0.33402777777777781</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <v>28</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="4">
         <v>-2.2222222222222223</v>
       </c>
       <c r="J8" s="3">
@@ -1447,10 +1450,10 @@
       <c r="G9" s="1">
         <v>0.30972222222222223</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <v>30</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="4">
         <v>-1.1111111111111112</v>
       </c>
       <c r="J9" s="3">
@@ -1523,10 +1526,10 @@
       <c r="G10" s="1">
         <v>3.9583333333333331E-2</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <v>32</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="4">
         <v>0</v>
       </c>
       <c r="J10" s="3">
@@ -1599,10 +1602,10 @@
       <c r="G11" s="1">
         <v>0.33749999999999997</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="4">
         <v>33</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="4">
         <v>0.55555555555555558</v>
       </c>
       <c r="J11" s="3">
@@ -1675,10 +1678,10 @@
       <c r="G12" s="1">
         <v>0.3125</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="4">
         <v>33</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="4">
         <v>0.55555555555555558</v>
       </c>
       <c r="J12" s="3">
@@ -1751,10 +1754,10 @@
       <c r="G13" s="1">
         <v>6.5277777777777782E-2</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>30</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="4">
         <v>-1.1111111111111112</v>
       </c>
       <c r="J13" s="3">
@@ -1827,10 +1830,10 @@
       <c r="G14" s="1">
         <v>0.4069444444444445</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="4">
         <v>30</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="4">
         <v>-1.1111111111111112</v>
       </c>
       <c r="J14" s="3">
@@ -1903,10 +1906,10 @@
       <c r="G15" s="1">
         <v>4.6527777777777779E-2</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="4">
         <v>17</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="4">
         <v>-8.3333333333333339</v>
       </c>
       <c r="J15" s="3">
@@ -1979,10 +1982,10 @@
       <c r="G16" s="1">
         <v>0.33749999999999997</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="4">
         <v>-2</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="4">
         <v>-18.888888888888889</v>
       </c>
       <c r="J16" s="3">
@@ -2055,10 +2058,10 @@
       <c r="G17" s="1">
         <v>0.15347222222222223</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
         <v>-3</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="4">
         <v>-19.444444444444443</v>
       </c>
       <c r="J17" s="3">
@@ -2131,10 +2134,10 @@
       <c r="G18" s="1">
         <v>0.29791666666666666</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="4">
         <v>3</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="4">
         <v>-16.111111111111111</v>
       </c>
       <c r="J18" s="3">
@@ -2207,10 +2210,10 @@
       <c r="G19" s="1">
         <v>0.30486111111111108</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="4">
         <v>2</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="4">
         <v>-16.666666666666668</v>
       </c>
       <c r="J19" s="3">
@@ -2283,10 +2286,10 @@
       <c r="G20" s="1">
         <v>0.3034722222222222</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="4">
         <v>18</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="4">
         <v>-7.7777777777777777</v>
       </c>
       <c r="J20" s="3">
@@ -2359,10 +2362,10 @@
       <c r="G21" s="1">
         <v>0.3</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>9</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="4">
         <v>-12.777777777777777</v>
       </c>
       <c r="J21" s="3">
@@ -2435,10 +2438,10 @@
       <c r="G22" s="1">
         <v>1.5277777777777777E-2</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="4">
         <v>2</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="4">
         <v>-16.666666666666668</v>
       </c>
       <c r="J22" s="3">
@@ -2511,10 +2514,10 @@
       <c r="G23" s="1">
         <v>7.6388888888888886E-3</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="4">
         <v>8</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="4">
         <v>-13.333333333333332</v>
       </c>
       <c r="J23" s="3">
@@ -2587,10 +2590,10 @@
       <c r="G24" s="1">
         <v>0.30694444444444441</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="4">
         <v>11</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="4">
         <v>-11.666666666666668</v>
       </c>
       <c r="J24" s="3">
@@ -2663,10 +2666,10 @@
       <c r="G25" s="1">
         <v>0.31458333333333333</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="4">
         <v>32</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="4">
         <v>0</v>
       </c>
       <c r="J25" s="3">
@@ -2739,10 +2742,10 @@
       <c r="G26" s="1">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="4">
         <v>33</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="4">
         <v>0.55555555555555558</v>
       </c>
       <c r="J26" s="3">
@@ -2815,10 +2818,10 @@
       <c r="G27" s="1">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="4">
         <v>36</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="4">
         <v>2.2222222222222223</v>
       </c>
       <c r="J27" s="3">
@@ -2891,10 +2894,10 @@
       <c r="G28" s="1">
         <v>0.25</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="4">
         <v>37</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="4">
         <v>2.7777777777777777</v>
       </c>
       <c r="J28" s="3">
@@ -2967,10 +2970,10 @@
       <c r="G29" s="1">
         <v>5.486111111111111E-2</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="4">
         <v>35</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="4">
         <v>1.6666666666666665</v>
       </c>
       <c r="J29" s="3">
@@ -3043,10 +3046,10 @@
       <c r="G30" s="1">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="4">
         <v>33</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="4">
         <v>0.55555555555555558</v>
       </c>
       <c r="J30" s="3">
@@ -3119,10 +3122,10 @@
       <c r="G31" s="1">
         <v>0.32222222222222224</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="4">
         <v>32</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="4">
         <v>0</v>
       </c>
       <c r="J31" s="3">
@@ -3195,10 +3198,10 @@
       <c r="G32" s="1">
         <v>0.32013888888888892</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="4">
         <v>32</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="4">
         <v>0</v>
       </c>
       <c r="J32" s="3">
@@ -3271,10 +3274,10 @@
       <c r="G33" s="1">
         <v>2.1527777777777781E-2</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="4">
         <v>33</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="4">
         <v>0.55555555555555558</v>
       </c>
       <c r="J33" s="3">
@@ -3347,10 +3350,10 @@
       <c r="G34" s="1">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="4">
         <v>36</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="4">
         <v>2.2222222222222223</v>
       </c>
       <c r="J34" s="3">
@@ -3423,10 +3426,10 @@
       <c r="G35" s="1">
         <v>0.3125</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="4">
         <v>30</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="4">
         <v>-1.1111111111111112</v>
       </c>
       <c r="J35" s="3">
@@ -3499,10 +3502,10 @@
       <c r="G36" s="1">
         <v>0.34097222222222223</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="4">
         <v>26</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="4">
         <v>-3.333333333333333</v>
       </c>
       <c r="J36" s="3">
@@ -3575,10 +3578,10 @@
       <c r="G37" s="1">
         <v>0.30763888888888891</v>
       </c>
-      <c r="H37" s="3">
-        <v>24</v>
-      </c>
-      <c r="I37" s="3">
+      <c r="H37" s="4">
+        <v>24</v>
+      </c>
+      <c r="I37" s="4">
         <v>-4.4444444444444446</v>
       </c>
       <c r="J37" s="3">
@@ -3651,10 +3654,10 @@
       <c r="G38" s="1">
         <v>0.3125</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="4">
         <v>26</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="4">
         <v>-3.333333333333333</v>
       </c>
       <c r="J38" s="3">
@@ -3727,10 +3730,10 @@
       <c r="G39" s="1">
         <v>6.2499999999999995E-3</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="4">
         <v>29</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="4">
         <v>-1.6666666666666665</v>
       </c>
       <c r="J39" s="3">
@@ -3803,10 +3806,10 @@
       <c r="G40" s="1">
         <v>0</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="4">
         <v>26</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="4">
         <v>-3.333333333333333</v>
       </c>
       <c r="J40" s="3">
@@ -3879,10 +3882,10 @@
       <c r="G41" s="1">
         <v>0.31875000000000003</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="4">
         <v>33</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="4">
         <v>0.55555555555555558</v>
       </c>
       <c r="J41" s="3">
@@ -3955,10 +3958,10 @@
       <c r="G42" s="1">
         <v>0.20416666666666669</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="4">
         <v>49</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="4">
         <v>9.4444444444444446</v>
       </c>
       <c r="J42" s="3">
@@ -4031,10 +4034,10 @@
       <c r="G43" s="1">
         <v>0.30416666666666664</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="4">
         <v>34</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="4">
         <v>1.1111111111111112</v>
       </c>
       <c r="J43" s="3">
@@ -4107,10 +4110,10 @@
       <c r="G44" s="1">
         <v>0.3215277777777778</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="4">
         <v>28</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="4">
         <v>-2.2222222222222223</v>
       </c>
       <c r="J44" s="3">
@@ -4183,10 +4186,10 @@
       <c r="G45" s="1">
         <v>0.3125</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="4">
         <v>28</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="4">
         <v>-2.2222222222222223</v>
       </c>
       <c r="J45" s="3">
@@ -4259,10 +4262,10 @@
       <c r="G46" s="1">
         <v>0.32916666666666666</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="4">
         <v>26</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="4">
         <v>-3.333333333333333</v>
       </c>
       <c r="J46" s="3">

</xml_diff>